<commit_message>
added sheet summarizing type of lithology and alluvium for each reach, to make it easy to read in and combine with other data.
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/Lithology of Redd Detection Study Reaches_Actual Final.xlsx
+++ b/analysis/data/raw_data/Lithology of Redd Detection Study Reaches_Actual Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seek/Documents/GitProjects/MyProjects/ReddObsErrThurow/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA627C7-601A-DD43-B7B3-80A13C3B4F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C8D614-D4E7-BC40-8755-0AA3765FC682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25580" windowHeight="18740" xr2:uid="{D7F3902F-D58B-4623-AAF8-8A308C793F7B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25580" windowHeight="18740" activeTab="1" xr2:uid="{D7F3902F-D58B-4623-AAF8-8A308C793F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,9 +186,6 @@
     <t>Alluvium</t>
   </si>
   <si>
-    <t>Lithology</t>
-  </si>
-  <si>
     <t>Beaver</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Lith</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A8CAB87-7953-42C0-AE24-E94DB1A35D22}">
   <dimension ref="A2:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1940,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7235E676-0E0D-294B-8852-8ACDD9946C8C}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1954,7 +1954,7 @@
         <v>48</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C1" s="42" t="s">
         <v>49</v>
@@ -1962,189 +1962,189 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="42">
         <v>5</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="42">
         <v>1</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="42">
         <v>5</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="42">
         <v>3</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="42">
         <v>2</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="42">
         <v>5</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="42">
         <v>5</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="42">
         <v>2</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="42">
         <v>2</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="42">
         <v>2</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="42">
         <v>5</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="42">
         <v>5</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="42">
         <v>2</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="42">
         <v>2</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="42">
         <v>1</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="42">
         <v>3</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="42">
         <v>5</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>